<commit_message>
New changes to UI
</commit_message>
<xml_diff>
--- a/Idei_Si_Principii/Guards.xlsx
+++ b/Idei_Si_Principii/Guards.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian Geanta\Documents\AndroidStudioProjects\SecurityPatrol\Idei_Si_Principii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian Geanta\StudioProjects\SecurityPatrol\Idei_Si_Principii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3CB970-78B0-40B8-8CB9-B1C2BB011B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5ECE8C-D8FA-4C87-B0F8-E131D838E007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3885" yWindow="3480" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Nume</t>
   </si>
@@ -44,16 +44,7 @@
     <t>Dumitru Marian</t>
   </si>
   <si>
-    <t>Adrian Geanta</t>
-  </si>
-  <si>
-    <t>Cosmin Geanta</t>
-  </si>
-  <si>
-    <t>Matei Marius</t>
-  </si>
-  <si>
-    <t>Matei Ioana</t>
+    <t>Popescu Ion</t>
   </si>
 </sst>
 </file>
@@ -444,7 +435,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,27 +475,21 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="4"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="4"/>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>

</xml_diff>